<commit_message>
pushing excel creation, upload, download code
</commit_message>
<xml_diff>
--- a/WebContent/WEB-INF/DataMappings.xlsx
+++ b/WebContent/WEB-INF/DataMappings.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rahul\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prash\gitbashnew2\All-in-One-FantasyGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,8 @@
   <sheets>
     <sheet name="TEAMNAMES" sheetId="1" r:id="rId1"/>
     <sheet name="TEAM_PLAYER_MAPPINGS" sheetId="2" r:id="rId2"/>
+    <sheet name="LEAGUE_RULES" sheetId="3" r:id="rId3"/>
+    <sheet name="GAMES" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="96">
   <si>
     <t>MUMBAI INDIANS</t>
   </si>
@@ -195,7 +197,124 @@
     <t>All-Rounder</t>
   </si>
   <si>
-    <t>Keeper/Batsman</t>
+    <t>RUNS</t>
+  </si>
+  <si>
+    <t>WICKETS</t>
+  </si>
+  <si>
+    <t>CATCHES</t>
+  </si>
+  <si>
+    <t>METRIC</t>
+  </si>
+  <si>
+    <t>LESS_THAN</t>
+  </si>
+  <si>
+    <t>GREATER_THAN</t>
+  </si>
+  <si>
+    <t>EQUALS</t>
+  </si>
+  <si>
+    <t>PER_SCORE</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>OPERATOR</t>
+  </si>
+  <si>
+    <t>SCORE</t>
+  </si>
+  <si>
+    <t>POINTS</t>
+  </si>
+  <si>
+    <t>RATIO</t>
+  </si>
+  <si>
+    <t>TEAM1</t>
+  </si>
+  <si>
+    <t>TEAM2</t>
+  </si>
+  <si>
+    <t>DATE( MM/DD/YYYY)</t>
+  </si>
+  <si>
+    <t>TIME(hh:mm:ss)</t>
+  </si>
+  <si>
+    <t>VENUE</t>
+  </si>
+  <si>
+    <t>MUMBAI</t>
+  </si>
+  <si>
+    <t>UNIQUE_ID</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>HS</t>
+  </si>
+  <si>
+    <t>LM</t>
+  </si>
+  <si>
+    <t>KP</t>
+  </si>
+  <si>
+    <t>MSD</t>
+  </si>
+  <si>
+    <t>RJ</t>
+  </si>
+  <si>
+    <t>DB</t>
+  </si>
+  <si>
+    <t>VK</t>
+  </si>
+  <si>
+    <t>ABdeV</t>
+  </si>
+  <si>
+    <t>SW</t>
+  </si>
+  <si>
+    <t>KLR</t>
+  </si>
+  <si>
+    <t>GG</t>
+  </si>
+  <si>
+    <t>YP</t>
+  </si>
+  <si>
+    <t>RU</t>
+  </si>
+  <si>
+    <t>SN</t>
+  </si>
+  <si>
+    <t>DW</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>BK</t>
+  </si>
+  <si>
+    <t>AN</t>
+  </si>
+  <si>
+    <t>WicketKeeper</t>
   </si>
 </sst>
 </file>
@@ -231,8 +350,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,7 +672,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -614,10 +736,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F07214C3-C036-4793-862C-845BE9B97262}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -627,7 +749,7 @@
     <col min="3" max="3" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>50</v>
       </c>
@@ -635,13 +757,16 @@
         <v>51</v>
       </c>
       <c r="C1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" t="s">
         <v>52</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -649,13 +774,16 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" t="s">
         <v>53</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -663,13 +791,16 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" t="s">
         <v>54</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -677,13 +808,16 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" t="s">
         <v>54</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -691,13 +825,16 @@
         <v>15</v>
       </c>
       <c r="C5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" t="s">
         <v>55</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -705,13 +842,16 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="D6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -719,13 +859,16 @@
         <v>19</v>
       </c>
       <c r="C7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" t="s">
         <v>55</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -733,13 +876,16 @@
         <v>21</v>
       </c>
       <c r="C8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" t="s">
         <v>55</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -747,13 +893,16 @@
         <v>23</v>
       </c>
       <c r="C9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" t="s">
         <v>53</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -761,13 +910,16 @@
         <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="D10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -775,13 +927,16 @@
         <v>27</v>
       </c>
       <c r="C11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" t="s">
         <v>55</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -789,13 +944,16 @@
         <v>29</v>
       </c>
       <c r="C12" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" t="s">
         <v>53</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -803,13 +961,16 @@
         <v>31</v>
       </c>
       <c r="C13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" t="s">
         <v>53</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -817,13 +978,16 @@
         <v>33</v>
       </c>
       <c r="C14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" t="s">
         <v>55</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -831,13 +995,16 @@
         <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
       <c r="D15" t="s">
+        <v>95</v>
+      </c>
+      <c r="E15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -845,13 +1012,16 @@
         <v>36</v>
       </c>
       <c r="C16" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" t="s">
         <v>54</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -859,13 +1029,16 @@
         <v>41</v>
       </c>
       <c r="C17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" t="s">
         <v>53</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -873,13 +1046,16 @@
         <v>43</v>
       </c>
       <c r="C18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" t="s">
         <v>53</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -887,13 +1063,16 @@
         <v>45</v>
       </c>
       <c r="C19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" t="s">
         <v>54</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -901,10 +1080,199 @@
         <v>47</v>
       </c>
       <c r="C20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D20" t="s">
         <v>54</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CF0FB42-DE70-4F46-B47B-095922A2514A}">
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14.109375" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" customWidth="1"/>
+    <col min="4" max="4" width="14.21875" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>-5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3">
+        <v>50</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C4" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2:A14" xr:uid="{F94AA79E-D2B3-47C1-AA5C-D6D4FC6303F1}">
+      <formula1>$A$16:$A$18</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B15" xr:uid="{513C84B1-0C1E-4D70-8D09-BA0BD66C3CC3}">
+      <formula1>$B$16:$B$18</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E15" xr:uid="{F9290EED-A4FB-43D3-B198-AB5D37296561}">
+      <formula1>$E$16:$E$17</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0011481B-8562-4525-B31F-A34C6FC50919}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="19.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2">
+        <v>43066</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2">
+        <v>43066</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E3" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>